<commit_message>
fix typos spotted by Aleah
</commit_message>
<xml_diff>
--- a/data/aurignacian-periods.xlsx
+++ b/data/aurignacian-periods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiecooper/Independent Research Study/SignBase/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Downloads/SignBase/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29507320-B411-8841-828B-EBA81E2C05D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F391AF0-6FC0-0C42-A290-7150D8DD7171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16600" xr2:uid="{79486DA5-00F7-8844-88EA-52FFFB3FA67C}"/>
+    <workbookView xWindow="7620" yWindow="760" windowWidth="21180" windowHeight="16600" xr2:uid="{79486DA5-00F7-8844-88EA-52FFFB3FA67C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -92,10 +91,10 @@
     <t>GI 8 - 6</t>
   </si>
   <si>
-    <t>Preceeded by Greenland Stadial 12, ends with GI 11</t>
-  </si>
-  <si>
     <t>Begins with Henrich Stadial 4, ends with GI 8</t>
+  </si>
+  <si>
+    <t>Preceded by Greenland Stadial 12, ends with GI 11</t>
   </si>
 </sst>
 </file>
@@ -473,7 +472,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,7 +508,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -537,7 +536,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">

</xml_diff>